<commit_message>
Update experimental setup script to make a single .ics calendar file with all experiments
</commit_message>
<xml_diff>
--- a/experimentalSetup.xlsx
+++ b/experimentalSetup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Dropbox (MIT)\reddien\bioscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{298AED80-7B8E-47A0-85DF-C9A00840748F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E9F54D-7D26-4DD5-A129-79365A1BE321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1_2" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="37">
   <si>
     <t>dates</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>pluck phx</t>
-  </si>
-  <si>
-    <t>fix 40</t>
   </si>
   <si>
     <t>bcat homeostatic</t>
@@ -129,9 +126,6 @@
     <t>Use a pipette tip to dispense liver in a thin line</t>
   </si>
   <si>
-    <t>wash if needed</t>
-  </si>
-  <si>
     <t>tlx-1 homeostatic</t>
   </si>
   <si>
@@ -142,6 +136,36 @@
   </si>
   <si>
     <t>Total worms: 480 (80 worms / experiment, 6 experiments)</t>
+  </si>
+  <si>
+    <t>Lucila: 6-8 weeks for ndk</t>
+  </si>
+  <si>
+    <t>fix 80</t>
+  </si>
+  <si>
+    <t>delayed fix (migraine)</t>
+  </si>
+  <si>
+    <t>delayed wash (migraine)</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>delayed fix (pharynges not developed yet)</t>
+  </si>
+  <si>
+    <t>fix 80 (10 dpa)</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>fix 40 (13 dpa - only controls fixed)</t>
+  </si>
+  <si>
+    <t>fix 40 (17 dpa - only experimental fixed)</t>
   </si>
 </sst>
 </file>
@@ -154,11 +178,25 @@
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -263,7 +301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -584,17 +622,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFCE181E"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFCE181E"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFFAA61A"/>
       </left>
@@ -679,108 +706,114 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" applyProtection="0">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="2" applyProtection="0">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="3" applyProtection="0">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="4" applyProtection="0">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="5" applyProtection="0">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="5" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="6" applyProtection="0">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="7" applyProtection="0">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="7" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="8" applyProtection="0">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="9" applyProtection="0">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="10" applyProtection="0">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="10" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="56">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="11" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="12" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="14" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="17" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="18" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="19" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="12" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="20" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="21" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="10" borderId="22" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="23" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="24" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="25" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="26" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="12" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="27" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="28" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="29" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="30" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="31" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="9" borderId="32" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="9" borderId="33" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="9" borderId="34" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="9" borderId="12" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="35" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="9" borderId="36" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="9" borderId="37" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="38" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="39" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="11" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="12" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="7" fillId="8" borderId="0" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="7" fillId="8" borderId="13" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="14" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="7" fillId="8" borderId="15" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="7" fillId="8" borderId="16" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="11" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="12" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="14" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="11" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="12" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="14" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="17" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="18" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="19" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="12" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="21" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="22" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="24" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="25" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="26" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="12" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="27" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="28" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="6" borderId="29" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="30" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="31" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="32" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="33" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="12" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="34" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="35" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="36" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="37" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="38" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="11" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="12" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="0" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="13" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="14" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="15" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="9" fillId="8" borderId="16" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="11" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="12" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="7" borderId="14" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="10" borderId="0" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="0" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
@@ -1182,10 +1215,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1201,295 +1234,324 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="36" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="38">
+        <v>44767</v>
+      </c>
+      <c r="C2" s="38">
+        <f t="shared" ref="C2:H8" si="0">B2+1</f>
+        <v>44768</v>
+      </c>
+      <c r="D2" s="38">
+        <f t="shared" si="0"/>
+        <v>44769</v>
+      </c>
+      <c r="E2" s="38">
+        <f t="shared" si="0"/>
+        <v>44770</v>
+      </c>
+      <c r="F2" s="38">
+        <f t="shared" si="0"/>
+        <v>44771</v>
+      </c>
+      <c r="G2" s="38">
+        <f t="shared" si="0"/>
+        <v>44772</v>
+      </c>
+      <c r="H2" s="39">
+        <f t="shared" si="0"/>
+        <v>44773</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="38">
+        <f t="shared" ref="B3:B8" si="1">H2+1</f>
+        <v>44774</v>
+      </c>
+      <c r="C3" s="38">
+        <f t="shared" si="0"/>
+        <v>44775</v>
+      </c>
+      <c r="D3" s="38">
+        <f t="shared" si="0"/>
+        <v>44776</v>
+      </c>
+      <c r="E3" s="38">
+        <f t="shared" si="0"/>
+        <v>44777</v>
+      </c>
+      <c r="F3" s="38">
+        <f t="shared" si="0"/>
+        <v>44778</v>
+      </c>
+      <c r="G3" s="38">
+        <f t="shared" si="0"/>
+        <v>44779</v>
+      </c>
+      <c r="H3" s="39">
+        <f t="shared" si="0"/>
+        <v>44780</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="38">
+        <f t="shared" si="1"/>
+        <v>44781</v>
+      </c>
+      <c r="C4" s="38">
+        <f t="shared" si="0"/>
+        <v>44782</v>
+      </c>
+      <c r="D4" s="38">
+        <f t="shared" si="0"/>
+        <v>44783</v>
+      </c>
+      <c r="E4" s="38">
+        <f t="shared" si="0"/>
+        <v>44784</v>
+      </c>
+      <c r="F4" s="38">
+        <f t="shared" si="0"/>
+        <v>44785</v>
+      </c>
+      <c r="G4" s="38">
+        <f t="shared" si="0"/>
+        <v>44786</v>
+      </c>
+      <c r="H4" s="39">
+        <f t="shared" si="0"/>
+        <v>44787</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="39">
-        <v>44767</v>
-      </c>
-      <c r="C2" s="39">
-        <f t="shared" ref="C2:H6" si="0">B2+1</f>
-        <v>44768</v>
-      </c>
-      <c r="D2" s="39">
-        <f t="shared" si="0"/>
-        <v>44769</v>
-      </c>
-      <c r="E2" s="39">
-        <f t="shared" si="0"/>
-        <v>44770</v>
-      </c>
-      <c r="F2" s="39">
-        <f t="shared" si="0"/>
-        <v>44771</v>
-      </c>
-      <c r="G2" s="39">
-        <f t="shared" si="0"/>
-        <v>44772</v>
-      </c>
-      <c r="H2" s="40">
-        <f t="shared" si="0"/>
-        <v>44773</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="39">
-        <f>H2+1</f>
-        <v>44774</v>
-      </c>
-      <c r="C3" s="39">
-        <f t="shared" si="0"/>
-        <v>44775</v>
-      </c>
-      <c r="D3" s="39">
-        <f t="shared" si="0"/>
-        <v>44776</v>
-      </c>
-      <c r="E3" s="39">
-        <f t="shared" si="0"/>
-        <v>44777</v>
-      </c>
-      <c r="F3" s="39">
-        <f t="shared" si="0"/>
-        <v>44778</v>
-      </c>
-      <c r="G3" s="39">
-        <f t="shared" si="0"/>
-        <v>44779</v>
-      </c>
-      <c r="H3" s="40">
-        <f t="shared" si="0"/>
-        <v>44780</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="39">
-        <f>H3+1</f>
-        <v>44781</v>
-      </c>
-      <c r="C4" s="39">
-        <f t="shared" si="0"/>
-        <v>44782</v>
-      </c>
-      <c r="D4" s="39">
-        <f t="shared" si="0"/>
-        <v>44783</v>
-      </c>
-      <c r="E4" s="39">
-        <f t="shared" si="0"/>
-        <v>44784</v>
-      </c>
-      <c r="F4" s="39">
-        <f t="shared" si="0"/>
-        <v>44785</v>
-      </c>
-      <c r="G4" s="39">
-        <f t="shared" si="0"/>
-        <v>44786</v>
-      </c>
-      <c r="H4" s="40">
-        <f t="shared" si="0"/>
-        <v>44787</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="39">
-        <f>H4+1</f>
+      <c r="B5" s="38">
+        <f t="shared" si="1"/>
         <v>44788</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="38">
         <f t="shared" si="0"/>
         <v>44789</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="38">
         <f t="shared" si="0"/>
         <v>44790</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="38">
         <f t="shared" si="0"/>
         <v>44791</v>
       </c>
-      <c r="F5" s="39">
+      <c r="F5" s="38">
         <f t="shared" si="0"/>
         <v>44792</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="38">
         <f t="shared" si="0"/>
         <v>44793</v>
       </c>
-      <c r="H5" s="40">
+      <c r="H5" s="39">
         <f t="shared" si="0"/>
         <v>44794</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="41">
+        <f t="shared" si="1"/>
+        <v>44795</v>
+      </c>
+      <c r="C6" s="41">
+        <f t="shared" si="0"/>
+        <v>44796</v>
+      </c>
+      <c r="D6" s="41">
+        <f t="shared" si="0"/>
+        <v>44797</v>
+      </c>
+      <c r="E6" s="41">
+        <f t="shared" si="0"/>
+        <v>44798</v>
+      </c>
+      <c r="F6" s="41">
+        <f t="shared" si="0"/>
+        <v>44799</v>
+      </c>
+      <c r="G6" s="41">
+        <f t="shared" si="0"/>
+        <v>44800</v>
+      </c>
+      <c r="H6" s="42">
+        <f t="shared" si="0"/>
+        <v>44801</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="42">
-        <f>H5+1</f>
-        <v>44795</v>
-      </c>
-      <c r="C6" s="42">
-        <f t="shared" si="0"/>
-        <v>44796</v>
-      </c>
-      <c r="D6" s="42">
-        <f t="shared" si="0"/>
-        <v>44797</v>
-      </c>
-      <c r="E6" s="42">
-        <f t="shared" si="0"/>
-        <v>44798</v>
-      </c>
-      <c r="F6" s="42">
-        <f t="shared" si="0"/>
-        <v>44799</v>
-      </c>
-      <c r="G6" s="42">
-        <f t="shared" si="0"/>
-        <v>44800</v>
-      </c>
-      <c r="H6" s="43">
-        <f t="shared" si="0"/>
-        <v>44801</v>
-      </c>
+    <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="38">
+        <f t="shared" si="1"/>
+        <v>44802</v>
+      </c>
+      <c r="C7" s="38">
+        <f t="shared" si="0"/>
+        <v>44803</v>
+      </c>
+      <c r="D7" s="38">
+        <f t="shared" si="0"/>
+        <v>44804</v>
+      </c>
+      <c r="E7" s="38">
+        <f t="shared" si="0"/>
+        <v>44805</v>
+      </c>
+      <c r="F7" s="38">
+        <f t="shared" si="0"/>
+        <v>44806</v>
+      </c>
+      <c r="G7" s="38">
+        <f t="shared" si="0"/>
+        <v>44807</v>
+      </c>
+      <c r="H7" s="38">
+        <f t="shared" si="0"/>
+        <v>44808</v>
+      </c>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="38">
+        <f t="shared" si="1"/>
+        <v>44809</v>
+      </c>
+      <c r="C8" s="38">
+        <f t="shared" si="0"/>
+        <v>44810</v>
+      </c>
+      <c r="D8" s="38">
+        <f t="shared" si="0"/>
+        <v>44811</v>
+      </c>
+      <c r="E8" s="38">
+        <f t="shared" si="0"/>
+        <v>44812</v>
+      </c>
+      <c r="F8" s="38">
+        <f t="shared" si="0"/>
+        <v>44813</v>
+      </c>
+      <c r="G8" s="38">
+        <f t="shared" si="0"/>
+        <v>44814</v>
+      </c>
+      <c r="H8" s="38">
+        <f t="shared" si="0"/>
+        <v>44815</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B10" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
@@ -1506,492 +1568,604 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C17" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D17" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E17" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="G17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H17" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>10</v>
-      </c>
       <c r="B18" s="12"/>
-      <c r="C18" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="C18" s="12"/>
       <c r="D18" s="12"/>
-      <c r="E18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="12" t="s">
+      <c r="B21" s="12"/>
+      <c r="C21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="22"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" s="21"/>
+      <c r="H27" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
+      <c r="G31" s="30"/>
+      <c r="H31" s="31"/>
+    </row>
+    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="30"/>
+      <c r="C32" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="30"/>
+      <c r="E32" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="30"/>
+      <c r="H32" s="31"/>
+    </row>
+    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="30"/>
+      <c r="G34" s="30"/>
+      <c r="H34" s="30"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22" s="18" t="s">
+      <c r="B35" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C37" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D37" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E37" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="18" t="s">
+      <c r="F37" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G37" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="H37" s="43" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="22"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F24" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="25"/>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="26"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="G27" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="H27" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="32"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="G29" s="31"/>
-      <c r="H29" s="32" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
-      <c r="G30" s="35" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="36"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="44" t="s">
-        <v>2</v>
-      </c>
-      <c r="D32" s="44" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>5</v>
-      </c>
-      <c r="G32" s="44" t="s">
-        <v>6</v>
-      </c>
-      <c r="H32" s="44" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="46"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="46"/>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="47"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="46"/>
-      <c r="C34" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="46"/>
-      <c r="E34" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="G34" s="46"/>
-      <c r="H34" s="46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="46"/>
-      <c r="C35" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="46"/>
-      <c r="E35" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="F35" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="G35" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="H35" s="46"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="B36" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="46"/>
-      <c r="E36" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="F36" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="49"/>
-      <c r="C37" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="46"/>
     </row>
     <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B39" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39" s="45"/>
+      <c r="C39" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="45"/>
+      <c r="C40" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H40" s="49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="45"/>
+      <c r="C41" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41" s="45"/>
+      <c r="H41" s="45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="48"/>
+      <c r="C42" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
+    </row>
+    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="44" t="s">
+      <c r="C44" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="44" t="s">
+      <c r="D44" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="44" t="s">
+      <c r="E44" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F39" s="44" t="s">
+      <c r="F44" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="44" t="s">
+      <c r="G44" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H39" s="44" t="s">
+      <c r="H44" s="43" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="45" t="s">
+    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="46"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="46"/>
-      <c r="E40" s="46"/>
-      <c r="F40" s="46"/>
-      <c r="G40" s="46"/>
-      <c r="H40" s="47"/>
-    </row>
-    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="45" t="s">
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="46"/>
+    </row>
+    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B41" s="46"/>
-      <c r="C41" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="46"/>
-      <c r="E41" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="F41" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="G41" s="46"/>
-      <c r="H41" s="46" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="45" t="s">
+      <c r="B46" s="45"/>
+      <c r="C46" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F46" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46" s="45"/>
+      <c r="H46" s="45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="46"/>
-      <c r="C42" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="F42" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="H42" s="46"/>
-    </row>
-    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="45" t="s">
+      <c r="B47" s="45"/>
+      <c r="C47" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D47" s="45"/>
+      <c r="E47" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F47" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" s="49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C43" s="46" t="s">
+      <c r="B48" s="45"/>
+      <c r="C48" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" s="45"/>
+      <c r="E48" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F48" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48" s="45"/>
+      <c r="H48" s="55" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="48"/>
+      <c r="C49" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="D43" s="46"/>
-      <c r="E43" s="46"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="46"/>
-      <c r="H43" s="46"/>
-    </row>
-    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="48" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="49"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="49"/>
-      <c r="E44" s="49"/>
-      <c r="F44" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" s="49"/>
-      <c r="H44" s="49"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
+      <c r="F49" s="48"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="48"/>
+    </row>
+    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="45"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
Update experimental setup tool to increment date by 1 when creating events for proper calendar entries
</commit_message>
<xml_diff>
--- a/experimentalSetup.xlsx
+++ b/experimentalSetup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Dropbox (MIT)\reddien\bioscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E9F54D-7D26-4DD5-A129-79365A1BE321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4E5EB8-9096-498F-AECE-FC6267D23B01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="15345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1_2" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="40">
   <si>
     <t>dates</t>
   </si>
@@ -165,7 +165,16 @@
     <t>fix 40 (13 dpa - only controls fixed)</t>
   </si>
   <si>
-    <t>fix 40 (17 dpa - only experimental fixed)</t>
+    <t>fix 20 whole worms (18 dpa - only experimental fixed)</t>
+  </si>
+  <si>
+    <t>delayed wash (vacation)</t>
+  </si>
+  <si>
+    <t>delayed pluck (migraine)</t>
+  </si>
+  <si>
+    <t>pluck 80</t>
   </si>
 </sst>
 </file>
@@ -178,11 +187,25 @@
     <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -706,113 +729,118 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" applyProtection="0">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" applyProtection="0">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="2" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="3" applyProtection="0">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="3" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="4" applyProtection="0">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="4" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="5" applyProtection="0">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="5" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="6" applyProtection="0">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="6" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="7" applyProtection="0">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="7" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" applyProtection="0">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="8" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" applyProtection="0">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="9" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="10" applyProtection="0">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="10" applyProtection="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="11" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="12" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="14" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="15" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="10" borderId="17" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="10" borderId="18" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="10" borderId="19" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="10" borderId="12" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="10" borderId="21" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="10" borderId="22" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="23" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="24" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="25" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="26" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="12" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="27" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="28" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="6" borderId="29" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="30" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="31" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="32" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="33" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="12" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="34" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="35" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="36" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="37" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="38" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="11" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="12" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="0" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="13" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="14" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="15" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="9" fillId="8" borderId="16" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="11" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="12" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="7" borderId="14" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="11" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="12" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="13" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="14" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="15" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="17" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="18" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="19" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="12" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="20" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="21" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="22" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="23" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="24" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="25" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="26" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="12" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="27" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="28" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="6" borderId="29" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="30" xfId="15" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="31" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="32" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="33" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="12" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="34" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="35" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="36" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="37" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="38" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="8" borderId="11" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="8" borderId="12" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="11" fillId="8" borderId="0" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="11" fillId="8" borderId="13" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="8" borderId="14" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="11" fillId="8" borderId="15" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="11" fillId="8" borderId="16" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="11" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="12" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="14" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="16" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="0" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="9" borderId="0" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="8" borderId="0" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="10" borderId="0" xfId="19" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="9" borderId="0" xfId="18" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="0" xfId="17" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="0" xfId="14" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="16" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="20">
@@ -1215,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1442,7 +1470,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="53" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="38">
@@ -1476,7 +1504,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="53" t="s">
         <v>34</v>
       </c>
       <c r="B8" s="38">
@@ -1615,75 +1643,79 @@
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="58" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B18" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C18" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E18" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G18" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H18" s="10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
-        <v>9</v>
-      </c>
       <c r="B19" s="12"/>
-      <c r="C19" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="C19" s="12"/>
       <c r="D19" s="12"/>
-      <c r="E19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>14</v>
-      </c>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
       <c r="G19" s="12"/>
-      <c r="H19" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="12"/>
       <c r="C20" s="12" t="s">
@@ -1696,16 +1728,14 @@
       <c r="F20" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G20" s="12" t="s">
-        <v>30</v>
-      </c>
+      <c r="G20" s="12"/>
       <c r="H20" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="12"/>
       <c r="C21" s="12" t="s">
@@ -1718,296 +1748,302 @@
       <c r="F21" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="12"/>
+      <c r="G21" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="H21" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="52" t="s">
+      <c r="B23" s="16"/>
+      <c r="C23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12" t="s">
+      <c r="B24" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="16"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="H25" s="12"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B27" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C27" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D27" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E27" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="F27" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="G27" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H25" s="19" t="s">
+      <c r="H27" s="19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="21"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="21"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="22"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="22"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F27" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G27" s="21"/>
-      <c r="H27" s="22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="24" t="s">
+      <c r="B29" s="21"/>
+      <c r="C29" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="21"/>
+      <c r="H29" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25" t="s">
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="25" t="s">
+      <c r="H30" s="25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
+    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B32" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C32" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D32" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E32" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="27" t="s">
+      <c r="F32" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="27" t="s">
+      <c r="G32" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="28" t="s">
+      <c r="H32" s="28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="31"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="32" t="s">
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="30"/>
+      <c r="E33" s="30"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="30"/>
+      <c r="H33" s="31"/>
+    </row>
+    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F32" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="30"/>
-      <c r="H32" s="31"/>
-    </row>
-    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34" t="s">
-        <v>29</v>
-      </c>
-      <c r="H33" s="35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="53" t="s">
-        <v>11</v>
-      </c>
       <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
+      <c r="C34" s="30" t="s">
+        <v>14</v>
+      </c>
       <c r="D34" s="30"/>
       <c r="E34" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="G34" s="30"/>
+      <c r="H34" s="31"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="34"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
+      <c r="G35" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="H35" s="35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="F34" s="30"/>
-      <c r="G34" s="30"/>
-      <c r="H34" s="30"/>
-    </row>
-    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="53" t="s">
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B37" s="30"/>
+      <c r="C37" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-    </row>
-    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="43" t="s">
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="43" t="s">
+      <c r="B39" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="43" t="s">
+      <c r="C39" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="43" t="s">
+      <c r="D39" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="43" t="s">
+      <c r="E39" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="43" t="s">
+      <c r="F39" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="43" t="s">
+      <c r="G39" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="43" t="s">
+      <c r="H39" s="43" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="45"/>
-      <c r="C38" s="45"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="46"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="45"/>
-      <c r="C39" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="F39" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="44" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B40" s="45"/>
-      <c r="C40" s="45" t="s">
-        <v>14</v>
-      </c>
+      <c r="C40" s="45"/>
       <c r="D40" s="45"/>
-      <c r="E40" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="F40" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="G40" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="H40" s="49" t="s">
-        <v>15</v>
-      </c>
+      <c r="E40" s="45"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="45"/>
+      <c r="H40" s="46"/>
     </row>
     <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="44" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B41" s="45"/>
       <c r="C41" s="45" t="s">
@@ -2026,146 +2062,238 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="47" t="s">
+      <c r="A42" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="45"/>
+      <c r="C42" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F42" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H42" s="49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="45"/>
+      <c r="C43" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F43" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="45"/>
+      <c r="H43" s="45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B42" s="48"/>
-      <c r="C42" s="50" t="s">
+      <c r="B44" s="48"/>
+      <c r="C44" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="48"/>
+      <c r="E44" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F44" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" s="48"/>
+      <c r="H44" s="56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="B45" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="D45" s="45"/>
+      <c r="E45" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-    </row>
-    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="B44" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="43" t="s">
-        <v>2</v>
-      </c>
-      <c r="D44" s="43" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" s="43" t="s">
-        <v>4</v>
-      </c>
-      <c r="F44" s="43" t="s">
-        <v>5</v>
-      </c>
-      <c r="G44" s="43" t="s">
-        <v>6</v>
-      </c>
-      <c r="H44" s="43" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
       <c r="F45" s="45"/>
       <c r="G45" s="45"/>
-      <c r="H45" s="46"/>
-    </row>
-    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" s="45"/>
-      <c r="C46" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="F46" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45" t="s">
-        <v>15</v>
-      </c>
+      <c r="H45" s="45"/>
     </row>
     <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="F47" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="G47" s="49" t="s">
-        <v>30</v>
-      </c>
-      <c r="H47" s="49" t="s">
-        <v>15</v>
+      <c r="A47" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="F47" s="43" t="s">
+        <v>5</v>
+      </c>
+      <c r="G47" s="43" t="s">
+        <v>6</v>
+      </c>
+      <c r="H47" s="43" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="45"/>
+      <c r="C48" s="45"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="46"/>
+    </row>
+    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B49" s="45"/>
+      <c r="C49" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F49" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G49" s="45"/>
+      <c r="H49" s="45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="45"/>
+      <c r="C50" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="F50" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="G50" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H50" s="49" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B48" s="45"/>
-      <c r="C48" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="D48" s="45"/>
-      <c r="E48" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="F48" s="49" t="s">
-        <v>14</v>
-      </c>
-      <c r="G48" s="45"/>
-      <c r="H48" s="55" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="47" t="s">
+      <c r="B51" s="45"/>
+      <c r="C51" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="D51" s="45"/>
+      <c r="E51" s="49" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" s="45"/>
+      <c r="H51" s="54" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="48"/>
-      <c r="C49" s="50" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="48"/>
-      <c r="H49" s="48"/>
-    </row>
-    <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="51" t="s">
+      <c r="B52" s="48"/>
+      <c r="C52" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="48"/>
+      <c r="E52" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" s="56" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" s="48"/>
+      <c r="H52" s="56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="B50" s="45"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="49" t="s">
+      <c r="B53" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C53" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" s="60" t="s">
+        <v>39</v>
+      </c>
+      <c r="E53" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="F53" s="49"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="45"/>
+    </row>
+    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="B54" s="45"/>
+      <c r="C54" s="49"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="60"/>
+      <c r="G54" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
+      <c r="H54" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>